<commit_message>
créations profils, extensions et datatype
Creation des profils :
TDDUIPatient et TDDUIPatientINS pour l'usager

Création de CodeSystem :
TDDUIIdentifer

Création DataType : 41585f601d0646487cbba93fdb2189a055e1934e
</commit_message>
<xml_diff>
--- a/302-contenu-fhir---ajout-des-données-usager/ig/StructureDefinition-fr-core-human-name.xlsx
+++ b/302-contenu-fhir---ajout-des-données-usager/ig/StructureDefinition-fr-core-human-name.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="168">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-07-10T14:59:37+00:00</t>
+    <t>2025-07-18T12:58:08+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -478,13 +478,10 @@
     <t>Part of the name that is acquired as a title due to academic, legal, employment or nobility status, etc. and that appears at the start of the name.</t>
   </si>
   <si>
-    <t>extensible</t>
-  </si>
-  <si>
     <t>Civilités des personnes physiques</t>
   </si>
   <si>
-    <t>https://mos.esante.gouv.fr/NOS/JDV_J78-Civilite-RASS/FHIR/JDV-J78-Civilite-RASS</t>
+    <t>https://mos.esante.gouv.fr/NOS/JDV_J245-Civilite-CISIS/FHIR/JDV-J245-Civilite-CISIS</t>
   </si>
   <si>
     <t>XPN.5</t>
@@ -872,7 +869,7 @@
     <col min="23" max="23" width="16.3203125" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="16.16796875" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="27.484375" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="64.01171875" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="65.7265625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="5.44140625" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="19.4765625" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="36.0390625" customWidth="true" bestFit="true"/>
@@ -1957,13 +1954,13 @@
         <v>76</v>
       </c>
       <c r="X10" t="s" s="2">
+        <v>118</v>
+      </c>
+      <c r="Y10" t="s" s="2">
         <v>150</v>
       </c>
-      <c r="Y10" t="s" s="2">
+      <c r="Z10" t="s" s="2">
         <v>151</v>
-      </c>
-      <c r="Z10" t="s" s="2">
-        <v>152</v>
       </c>
       <c r="AA10" t="s" s="2">
         <v>76</v>
@@ -1996,21 +1993,21 @@
         <v>84</v>
       </c>
       <c r="AK10" t="s" s="2">
+        <v>152</v>
+      </c>
+      <c r="AL10" t="s" s="2">
         <v>153</v>
       </c>
-      <c r="AL10" t="s" s="2">
+      <c r="AM10" t="s" s="2">
         <v>154</v>
-      </c>
-      <c r="AM10" t="s" s="2">
-        <v>155</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" t="s" s="2">
@@ -2036,10 +2033,10 @@
         <v>90</v>
       </c>
       <c r="L11" t="s" s="2">
+        <v>156</v>
+      </c>
+      <c r="M11" t="s" s="2">
         <v>157</v>
-      </c>
-      <c r="M11" t="s" s="2">
-        <v>158</v>
       </c>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
@@ -2090,7 +2087,7 @@
         <v>76</v>
       </c>
       <c r="AF11" t="s" s="2">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AG11" t="s" s="2">
         <v>77</v>
@@ -2105,10 +2102,10 @@
         <v>84</v>
       </c>
       <c r="AK11" t="s" s="2">
+        <v>158</v>
+      </c>
+      <c r="AL11" t="s" s="2">
         <v>159</v>
-      </c>
-      <c r="AL11" t="s" s="2">
-        <v>160</v>
       </c>
       <c r="AM11" t="s" s="2">
         <v>76</v>
@@ -2116,10 +2113,10 @@
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" t="s" s="2">
@@ -2142,17 +2139,17 @@
         <v>112</v>
       </c>
       <c r="K12" t="s" s="2">
+        <v>161</v>
+      </c>
+      <c r="L12" t="s" s="2">
         <v>162</v>
       </c>
-      <c r="L12" t="s" s="2">
+      <c r="M12" t="s" s="2">
         <v>163</v>
-      </c>
-      <c r="M12" t="s" s="2">
-        <v>164</v>
       </c>
       <c r="N12" s="2"/>
       <c r="O12" t="s" s="2">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="P12" t="s" s="2">
         <v>76</v>
@@ -2201,7 +2198,7 @@
         <v>76</v>
       </c>
       <c r="AF12" t="s" s="2">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AG12" t="s" s="2">
         <v>77</v>
@@ -2216,13 +2213,13 @@
         <v>84</v>
       </c>
       <c r="AK12" t="s" s="2">
+        <v>165</v>
+      </c>
+      <c r="AL12" t="s" s="2">
         <v>166</v>
       </c>
-      <c r="AL12" t="s" s="2">
+      <c r="AM12" t="s" s="2">
         <v>167</v>
-      </c>
-      <c r="AM12" t="s" s="2">
-        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>